<commit_message>
Updated spelling of Morocco
</commit_message>
<xml_diff>
--- a/docs/requirements/Master Data Tables - Test Data/master-location.xlsx
+++ b/docs/requirements/Master Data Tables - Test Data/master-location.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip\docs\requirements\Master Data Tables - Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1045476\Documents\GitHub\mosip\docs\requirements\Master Data Tables - Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885BF720-0CF6-42BC-AB54-7EFAF25E93D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{962DCE18-D4A9-4E5E-8F8F-502EB48250F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>MOR</t>
   </si>
   <si>
-    <t>Morroco</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>RAB</t>
+  </si>
+  <si>
+    <t>Morocco</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1141,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1183,25 +1185,25 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1209,25 +1211,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
       <c r="G3" t="b">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1235,373 +1237,373 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
       <c r="G4" t="b">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>22</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>26</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
         <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1615,22 +1617,22 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1644,22 +1646,22 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1673,109 +1675,109 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
         <v>43</v>
-      </c>
-      <c r="B20" t="s">
-        <v>44</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1789,22 +1791,22 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23" t="b">
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1818,22 +1820,22 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G24" t="b">
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1847,109 +1849,109 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" t="s">
         <v>42</v>
       </c>
-      <c r="E25" t="s">
-        <v>43</v>
-      </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G25" t="b">
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
         <v>46</v>
-      </c>
-      <c r="B26" t="s">
-        <v>47</v>
       </c>
       <c r="C26">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
         <v>46</v>
-      </c>
-      <c r="B28" t="s">
-        <v>47</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G28" t="b">
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1963,22 +1965,22 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -1992,22 +1994,22 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -2021,109 +2023,109 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G31" t="b">
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
         <v>49</v>
-      </c>
-      <c r="B32" t="s">
-        <v>50</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G32" t="b">
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G33" t="b">
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
         <v>49</v>
-      </c>
-      <c r="B34" t="s">
-        <v>50</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G34" t="b">
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -2137,22 +2139,22 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G35" t="b">
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -2166,22 +2168,22 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -2195,109 +2197,109 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" t="s">
         <v>52</v>
-      </c>
-      <c r="B38" t="s">
-        <v>53</v>
       </c>
       <c r="C38">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G38" t="b">
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39">
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G39" t="b">
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
         <v>52</v>
-      </c>
-      <c r="B40" t="s">
-        <v>53</v>
       </c>
       <c r="C40">
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
       </c>
       <c r="H40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -2311,22 +2313,22 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G41" t="b">
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -2340,22 +2342,22 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G42" t="b">
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -2369,109 +2371,109 @@
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G43" t="b">
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" t="s">
         <v>55</v>
-      </c>
-      <c r="B44" t="s">
-        <v>56</v>
       </c>
       <c r="C44">
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45">
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G45" t="b">
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" t="s">
         <v>55</v>
-      </c>
-      <c r="B46" t="s">
-        <v>56</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G46" t="b">
         <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -2485,22 +2487,22 @@
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G47" t="b">
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -2514,22 +2516,22 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G48" t="b">
         <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
@@ -2543,109 +2545,109 @@
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G49" t="b">
         <v>1</v>
       </c>
       <c r="H49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" t="s">
         <v>58</v>
-      </c>
-      <c r="B50" t="s">
-        <v>59</v>
       </c>
       <c r="C50">
         <v>4</v>
       </c>
       <c r="D50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G50" t="b">
         <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C51">
         <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G51" t="b">
         <v>1</v>
       </c>
       <c r="H51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" t="s">
         <v>58</v>
-      </c>
-      <c r="B52" t="s">
-        <v>59</v>
       </c>
       <c r="C52">
         <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G52" t="b">
         <v>1</v>
       </c>
       <c r="H52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
@@ -2659,22 +2661,22 @@
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G53" t="b">
         <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
@@ -2688,22 +2690,22 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G54" t="b">
         <v>1</v>
       </c>
       <c r="H54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
@@ -2717,109 +2719,109 @@
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G55" t="b">
         <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" t="s">
         <v>61</v>
-      </c>
-      <c r="B56" t="s">
-        <v>62</v>
       </c>
       <c r="C56">
         <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G56" t="b">
         <v>1</v>
       </c>
       <c r="H56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C57">
         <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G57" t="b">
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
         <v>61</v>
-      </c>
-      <c r="B58" t="s">
-        <v>62</v>
       </c>
       <c r="C58">
         <v>4</v>
       </c>
       <c r="D58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G58" t="b">
         <v>1</v>
       </c>
       <c r="H58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
@@ -2833,22 +2835,22 @@
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G59" t="b">
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
@@ -2862,22 +2864,22 @@
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G60" t="b">
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
@@ -2891,283 +2893,283 @@
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G61" t="b">
         <v>1</v>
       </c>
       <c r="H61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" t="s">
         <v>64</v>
-      </c>
-      <c r="B62" t="s">
-        <v>65</v>
       </c>
       <c r="C62">
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G62" t="b">
         <v>1</v>
       </c>
       <c r="H62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63">
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G63" t="b">
         <v>1</v>
       </c>
       <c r="H63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
         <v>64</v>
-      </c>
-      <c r="B64" t="s">
-        <v>65</v>
       </c>
       <c r="C64">
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G64" t="b">
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65">
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F65" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G65" t="b">
         <v>1</v>
       </c>
       <c r="H65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C66">
         <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G66" t="b">
         <v>1</v>
       </c>
       <c r="H66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C67">
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G67" t="b">
         <v>1</v>
       </c>
       <c r="H67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
         <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>68</v>
       </c>
       <c r="C68">
         <v>4</v>
       </c>
       <c r="D68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G68" t="b">
         <v>1</v>
       </c>
       <c r="H68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C69">
         <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E69" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G69" t="b">
         <v>1</v>
       </c>
       <c r="H69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" t="s">
         <v>67</v>
-      </c>
-      <c r="B70" t="s">
-        <v>68</v>
       </c>
       <c r="C70">
         <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G70" t="b">
         <v>1</v>
       </c>
       <c r="H70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I70" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -3181,22 +3183,22 @@
         <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G71" t="b">
         <v>1</v>
       </c>
       <c r="H71" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
@@ -3210,22 +3212,22 @@
         <v>5</v>
       </c>
       <c r="D72" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E72" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G72" t="b">
         <v>1</v>
       </c>
       <c r="H72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -3239,109 +3241,109 @@
         <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E73" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F73" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G73" t="b">
         <v>1</v>
       </c>
       <c r="H73" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>69</v>
+      </c>
+      <c r="B74" t="s">
         <v>70</v>
-      </c>
-      <c r="B74" t="s">
-        <v>71</v>
       </c>
       <c r="C74">
         <v>4</v>
       </c>
       <c r="D74" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F74" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G74" t="b">
         <v>1</v>
       </c>
       <c r="H74" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C75">
         <v>4</v>
       </c>
       <c r="D75" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G75" t="b">
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
+        <v>69</v>
+      </c>
+      <c r="B76" t="s">
         <v>70</v>
-      </c>
-      <c r="B76" t="s">
-        <v>71</v>
       </c>
       <c r="C76">
         <v>4</v>
       </c>
       <c r="D76" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E76" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G76" t="b">
         <v>1</v>
       </c>
       <c r="H76" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I76" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
@@ -3355,22 +3357,22 @@
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F77" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G77" t="b">
         <v>1</v>
       </c>
       <c r="H77" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I77" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
@@ -3384,22 +3386,22 @@
         <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G78" t="b">
         <v>1</v>
       </c>
       <c r="H78" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
@@ -3413,109 +3415,109 @@
         <v>5</v>
       </c>
       <c r="D79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E79" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F79" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G79" t="b">
         <v>1</v>
       </c>
       <c r="H79" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" t="s">
         <v>73</v>
-      </c>
-      <c r="B80" t="s">
-        <v>74</v>
       </c>
       <c r="C80">
         <v>4</v>
       </c>
       <c r="D80" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F80" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G80" t="b">
         <v>1</v>
       </c>
       <c r="H80" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I80" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C81">
         <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E81" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G81" t="b">
         <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I81" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>72</v>
+      </c>
+      <c r="B82" t="s">
         <v>73</v>
-      </c>
-      <c r="B82" t="s">
-        <v>74</v>
       </c>
       <c r="C82">
         <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F82" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G82" t="b">
         <v>1</v>
       </c>
       <c r="H82" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I82" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -3529,22 +3531,22 @@
         <v>5</v>
       </c>
       <c r="D83" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E83" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F83" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G83" t="b">
         <v>1</v>
       </c>
       <c r="H83" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
@@ -3558,22 +3560,22 @@
         <v>5</v>
       </c>
       <c r="D84" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E84" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G84" t="b">
         <v>1</v>
       </c>
       <c r="H84" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I84" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
@@ -3587,109 +3589,109 @@
         <v>5</v>
       </c>
       <c r="D85" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E85" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F85" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G85" t="b">
         <v>1</v>
       </c>
       <c r="H85" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I85" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>75</v>
+      </c>
+      <c r="B86" t="s">
         <v>76</v>
-      </c>
-      <c r="B86" t="s">
-        <v>77</v>
       </c>
       <c r="C86">
         <v>4</v>
       </c>
       <c r="D86" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E86" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F86" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G86" t="b">
         <v>1</v>
       </c>
       <c r="H86" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B87" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C87">
         <v>4</v>
       </c>
       <c r="D87" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E87" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G87" t="b">
         <v>1</v>
       </c>
       <c r="H87" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I87" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>75</v>
+      </c>
+      <c r="B88" t="s">
         <v>76</v>
-      </c>
-      <c r="B88" t="s">
-        <v>77</v>
       </c>
       <c r="C88">
         <v>4</v>
       </c>
       <c r="D88" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E88" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F88" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G88" t="b">
         <v>1</v>
       </c>
       <c r="H88" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I88" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -3703,22 +3705,22 @@
         <v>5</v>
       </c>
       <c r="D89" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F89" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G89" t="b">
         <v>1</v>
       </c>
       <c r="H89" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I89" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -3732,22 +3734,22 @@
         <v>5</v>
       </c>
       <c r="D90" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E90" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F90" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G90" t="b">
         <v>1</v>
       </c>
       <c r="H90" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I90" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
@@ -3761,109 +3763,109 @@
         <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E91" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F91" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G91" t="b">
         <v>1</v>
       </c>
       <c r="H91" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I91" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>78</v>
+      </c>
+      <c r="B92" t="s">
         <v>79</v>
-      </c>
-      <c r="B92" t="s">
-        <v>80</v>
       </c>
       <c r="C92">
         <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E92" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F92" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G92" t="b">
         <v>1</v>
       </c>
       <c r="H92" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I92" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B93" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C93">
         <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F93" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G93" t="b">
         <v>1</v>
       </c>
       <c r="H93" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I93" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
+        <v>78</v>
+      </c>
+      <c r="B94" t="s">
         <v>79</v>
-      </c>
-      <c r="B94" t="s">
-        <v>80</v>
       </c>
       <c r="C94">
         <v>4</v>
       </c>
       <c r="D94" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F94" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G94" t="b">
         <v>1</v>
       </c>
       <c r="H94" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I94" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
@@ -3877,22 +3879,22 @@
         <v>5</v>
       </c>
       <c r="D95" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E95" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F95" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G95" t="b">
         <v>1</v>
       </c>
       <c r="H95" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I95" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
@@ -3906,22 +3908,22 @@
         <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E96" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G96" t="b">
         <v>1</v>
       </c>
       <c r="H96" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I96" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
@@ -3935,109 +3937,109 @@
         <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E97" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F97" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G97" t="b">
         <v>1</v>
       </c>
       <c r="H97" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I97" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
+        <v>81</v>
+      </c>
+      <c r="B98" t="s">
         <v>82</v>
-      </c>
-      <c r="B98" t="s">
-        <v>83</v>
       </c>
       <c r="C98">
         <v>4</v>
       </c>
       <c r="D98" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E98" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F98" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G98" t="b">
         <v>1</v>
       </c>
       <c r="H98" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I98" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B99" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C99">
         <v>4</v>
       </c>
       <c r="D99" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E99" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G99" t="b">
         <v>1</v>
       </c>
       <c r="H99" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I99" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B100" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C100">
         <v>4</v>
       </c>
       <c r="D100" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E100" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F100" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G100" t="b">
         <v>1</v>
       </c>
       <c r="H100" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I100" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
@@ -4051,22 +4053,22 @@
         <v>5</v>
       </c>
       <c r="D101" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E101" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F101" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G101" t="b">
         <v>1</v>
       </c>
       <c r="H101" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I101" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
@@ -4080,22 +4082,22 @@
         <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E102" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G102" t="b">
         <v>1</v>
       </c>
       <c r="H102" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I102" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
@@ -4109,109 +4111,109 @@
         <v>5</v>
       </c>
       <c r="D103" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E103" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F103" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G103" t="b">
         <v>1</v>
       </c>
       <c r="H103" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I103" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>85</v>
+      </c>
+      <c r="B104" t="s">
         <v>86</v>
-      </c>
-      <c r="B104" t="s">
-        <v>87</v>
       </c>
       <c r="C104">
         <v>4</v>
       </c>
       <c r="D104" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F104" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G104" t="b">
         <v>1</v>
       </c>
       <c r="H104" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I104" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B105" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C105">
         <v>4</v>
       </c>
       <c r="D105" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E105" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F105" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G105" t="b">
         <v>1</v>
       </c>
       <c r="H105" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I105" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>85</v>
+      </c>
+      <c r="B106" t="s">
         <v>86</v>
-      </c>
-      <c r="B106" t="s">
-        <v>87</v>
       </c>
       <c r="C106">
         <v>4</v>
       </c>
       <c r="D106" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E106" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F106" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G106" t="b">
         <v>1</v>
       </c>
       <c r="H106" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I106" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
@@ -4225,22 +4227,22 @@
         <v>5</v>
       </c>
       <c r="D107" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E107" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F107" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G107" t="b">
         <v>1</v>
       </c>
       <c r="H107" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I107" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
@@ -4254,22 +4256,22 @@
         <v>5</v>
       </c>
       <c r="D108" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E108" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G108" t="b">
         <v>1</v>
       </c>
       <c r="H108" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I108" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
@@ -4283,22 +4285,22 @@
         <v>5</v>
       </c>
       <c r="D109" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F109" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G109" t="b">
         <v>1</v>
       </c>
       <c r="H109" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I109" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
@@ -4312,22 +4314,22 @@
         <v>5</v>
       </c>
       <c r="D110" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E110" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F110" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G110" t="b">
         <v>1</v>
       </c>
       <c r="H110" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I110" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
@@ -4341,22 +4343,22 @@
         <v>5</v>
       </c>
       <c r="D111" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E111" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F111" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G111" t="b">
         <v>1</v>
       </c>
       <c r="H111" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I111" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
@@ -4370,22 +4372,22 @@
         <v>5</v>
       </c>
       <c r="D112" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E112" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F112" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G112" t="b">
         <v>1</v>
       </c>
       <c r="H112" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I112" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
@@ -4399,22 +4401,22 @@
         <v>5</v>
       </c>
       <c r="D113" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E113" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F113" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G113" t="b">
         <v>1</v>
       </c>
       <c r="H113" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I113" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
@@ -4428,22 +4430,22 @@
         <v>5</v>
       </c>
       <c r="D114" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E114" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F114" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G114" t="b">
         <v>1</v>
       </c>
       <c r="H114" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I114" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
@@ -4457,22 +4459,22 @@
         <v>5</v>
       </c>
       <c r="D115" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E115" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F115" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G115" t="b">
         <v>1</v>
       </c>
       <c r="H115" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I115" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
@@ -4486,22 +4488,22 @@
         <v>5</v>
       </c>
       <c r="D116" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E116" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F116" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G116" t="b">
         <v>1</v>
       </c>
       <c r="H116" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I116" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
@@ -4515,22 +4517,22 @@
         <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E117" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F117" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G117" t="b">
         <v>1</v>
       </c>
       <c r="H117" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I117" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
@@ -4544,22 +4546,22 @@
         <v>5</v>
       </c>
       <c r="D118" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E118" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G118" t="b">
         <v>1</v>
       </c>
       <c r="H118" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I118" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
@@ -4573,22 +4575,22 @@
         <v>5</v>
       </c>
       <c r="D119" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E119" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F119" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G119" t="b">
         <v>1</v>
       </c>
       <c r="H119" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I119" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>